<commit_message>
actualizando grupos de trabajo
</commit_message>
<xml_diff>
--- a/documentacion-proyecto-final/Lista de Grupos.xlsx
+++ b/documentacion-proyecto-final/Lista de Grupos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodiGo\codigo-virtual-6\documentacion-proyecto-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17A9CA85-7E48-4BB1-873E-1FFED6B1508E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35182FE-E7BF-45A2-82A2-F455D554B326}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FBBCDA62-F49D-4479-AC97-88D87F0AB5BA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="119">
   <si>
     <t>N°</t>
   </si>
@@ -355,6 +355,36 @@
   </si>
   <si>
     <t>Grupo</t>
+  </si>
+  <si>
+    <t>Proyecto</t>
+  </si>
+  <si>
+    <t>Ecommerce para pymes</t>
+  </si>
+  <si>
+    <t>PROYECTO WASIO place</t>
+  </si>
+  <si>
+    <t>Proyecto personal</t>
+  </si>
+  <si>
+    <t>iTek</t>
+  </si>
+  <si>
+    <t>MIFIT TEMPO</t>
+  </si>
+  <si>
+    <t>CHACHI</t>
+  </si>
+  <si>
+    <t>LOSTPET</t>
+  </si>
+  <si>
+    <t>Ecommerce informatico</t>
+  </si>
+  <si>
+    <t>No presentó</t>
   </si>
 </sst>
 </file>
@@ -399,7 +429,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +475,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -611,9 +671,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -648,9 +705,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -695,6 +749,98 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1009,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E28C75B-B812-44F5-A425-98423DE35478}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,9 +1171,10 @@
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="29.42578125" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,634 +1199,715 @@
       <c r="H1" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F2" s="8">
-        <v>947375704</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="48">
+        <v>990378205</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="46">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="85" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F3" s="8">
-        <v>990378205</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="48">
+        <v>900585236</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="46">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="8">
-        <v>900585236</v>
-      </c>
-      <c r="G4" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="48">
+        <v>64</v>
+      </c>
+      <c r="F4" s="9">
+        <v>983721679</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="46">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="9">
-        <v>983721679</v>
-      </c>
-      <c r="G5" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>16</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="14">
+        <v>996534622</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="47">
+        <v>2</v>
+      </c>
+      <c r="I5" s="47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>67</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="14">
-        <v>996534622</v>
-      </c>
-      <c r="G6" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="49">
+        <v>71</v>
+      </c>
+      <c r="F6" s="16">
+        <v>970318010</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="47">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F7" s="16">
-        <v>970318010</v>
-      </c>
-      <c r="G7" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" s="49">
+        <v>972696048</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="47">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="16">
-        <v>972696048</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="H8" s="49">
+        <v>87</v>
+      </c>
+      <c r="F8" s="15">
+        <v>994455997</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="47">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" s="15">
-        <v>994455997</v>
-      </c>
-      <c r="G9" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="49">
+        <v>106</v>
+      </c>
+      <c r="F9" s="16">
+        <v>982388953</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="47">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
-        <v>26</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="16">
-        <v>982388953</v>
-      </c>
-      <c r="G10" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" s="49">
+      <c r="I9" s="47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17">
+        <v>6</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="20">
+        <v>942176798</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="48">
+        <v>3</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
+        <v>23</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="20">
+        <v>959692129</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="48">
+        <v>3</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22">
+        <v>4</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="26">
+        <v>935212401</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="49">
+        <v>4</v>
+      </c>
+      <c r="I12" s="49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22">
+        <v>7</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="27">
+        <v>996998808</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="49">
+        <v>4</v>
+      </c>
+      <c r="I13" s="49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22">
+        <v>11</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="26">
+        <v>994955279</v>
+      </c>
+      <c r="G14" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="49">
+        <v>4</v>
+      </c>
+      <c r="I14" s="86" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22">
+        <v>13</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="27">
+        <v>946712465</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="49">
+        <v>4</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="28">
+        <v>19</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="32">
+        <v>998238959</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="50">
+        <v>5</v>
+      </c>
+      <c r="I16" s="50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28">
+        <v>25</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="33">
+        <v>983315423</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="50">
+        <v>5</v>
+      </c>
+      <c r="I17" s="50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28">
+        <v>10</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="33">
+        <v>993096628</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="50">
+        <v>5</v>
+      </c>
+      <c r="I18" s="50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34">
+        <v>12</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="37">
+        <v>997334727</v>
+      </c>
+      <c r="G19" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="51">
+        <v>6</v>
+      </c>
+      <c r="I19" s="51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34">
+        <v>3</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="37">
+        <v>926569656</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="51">
+        <v>6</v>
+      </c>
+      <c r="I20" s="51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="34">
+        <v>20</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="39">
+        <v>976124099</v>
+      </c>
+      <c r="G21" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="51">
+        <v>6</v>
+      </c>
+      <c r="I21" s="51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="34">
+        <v>22</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="37">
+        <v>939802475</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="51">
+        <v>6</v>
+      </c>
+      <c r="I22" s="87" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="52">
+        <v>1</v>
+      </c>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="55">
+        <v>948098851</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="57">
+        <v>7</v>
+      </c>
+      <c r="I23" s="57" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="58">
+        <v>9</v>
+      </c>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="61">
+        <v>934505545</v>
+      </c>
+      <c r="G24" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="63">
+        <v>8</v>
+      </c>
+      <c r="I24" s="63" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="64">
+        <v>24</v>
+      </c>
+      <c r="B25" s="65"/>
+      <c r="C25" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="68">
+        <v>948901251</v>
+      </c>
+      <c r="G25" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="70">
+        <v>9</v>
+      </c>
+      <c r="I25" s="70" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="71">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
-        <v>6</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="20">
-        <v>942176798</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17">
-        <v>23</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="20">
-        <v>959692129</v>
-      </c>
-      <c r="G12" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="H12" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
-        <v>24</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="20">
-        <v>948901251</v>
-      </c>
-      <c r="G13" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
-        <v>1</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="22">
-        <v>948098851</v>
-      </c>
-      <c r="G14" s="44" t="s">
+      <c r="B26" s="72"/>
+      <c r="C26" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="75">
+        <v>947375704</v>
+      </c>
+      <c r="G26" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="77">
         <v>10</v>
       </c>
-      <c r="H14" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23">
-        <v>4</v>
-      </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="27">
-        <v>935212401</v>
-      </c>
-      <c r="G15" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23">
-        <v>7</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="28">
-        <v>996998808</v>
-      </c>
-      <c r="G16" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23">
+      <c r="I26" s="77" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="78">
+        <v>14</v>
+      </c>
+      <c r="B27" s="79"/>
+      <c r="C27" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="81" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="82">
+        <v>914342202</v>
+      </c>
+      <c r="G27" s="83" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="84">
         <v>11</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="27">
-        <v>994955279</v>
-      </c>
-      <c r="G17" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23">
-        <v>13</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="28">
-        <v>946712465</v>
-      </c>
-      <c r="G18" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23">
-        <v>14</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="27">
-        <v>914342202</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" s="51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29">
-        <v>19</v>
-      </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="33">
-        <v>998238959</v>
-      </c>
-      <c r="G20" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" s="52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="29">
-        <v>25</v>
-      </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="34">
-        <v>983315423</v>
-      </c>
-      <c r="G21" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="29">
-        <v>9</v>
-      </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="35">
-        <v>934505545</v>
-      </c>
-      <c r="G22" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="29">
-        <v>10</v>
-      </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="34">
-        <v>993096628</v>
-      </c>
-      <c r="G23" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" s="52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="36">
-        <v>12</v>
-      </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="39">
-        <v>997334727</v>
-      </c>
-      <c r="G24" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24" s="53">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36">
-        <v>3</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="39">
-        <v>926569656</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="53">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36">
-        <v>20</v>
-      </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="41">
-        <v>976124099</v>
-      </c>
-      <c r="G26" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" s="53">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="36">
-        <v>22</v>
-      </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" s="39">
-        <v>939802475</v>
-      </c>
-      <c r="G27" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" s="53">
-        <v>6</v>
+      <c r="I27" s="84" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{C3DEB505-0AC6-45E4-A5E3-7A669D77B163}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H27">
+  <autoFilter ref="A1:I1" xr:uid="{4C26A0E5-1A56-4574-8BA0-EAEE7463E728}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I27">
       <sortCondition ref="H1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
agregando nuevo listado de grupos
</commit_message>
<xml_diff>
--- a/documentacion-proyecto-final/Lista de Grupos.xlsx
+++ b/documentacion-proyecto-final/Lista de Grupos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodiGo\codigo-virtual-6\documentacion-proyecto-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35182FE-E7BF-45A2-82A2-F455D554B326}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7072B17A-1624-4E3B-BD1F-DA56AA376689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FBBCDA62-F49D-4479-AC97-88D87F0AB5BA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="120">
   <si>
     <t>N°</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>No presentó</t>
+  </si>
+  <si>
+    <t>GeoRent</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +508,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -606,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -667,9 +676,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -840,7 +846,26 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1158,7 +1183,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,13 +1245,13 @@
       <c r="F2" s="8">
         <v>990378205</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="46">
+      <c r="H2" s="45">
         <v>1</v>
       </c>
-      <c r="I2" s="85" t="s">
+      <c r="I2" s="84" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1247,13 +1272,13 @@
       <c r="F3" s="8">
         <v>900585236</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>1</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="45" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1274,13 +1299,13 @@
       <c r="F4" s="9">
         <v>983721679</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>1</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="45" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1301,13 +1326,13 @@
       <c r="F5" s="14">
         <v>996534622</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="46">
         <v>2</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="46" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1328,13 +1353,13 @@
       <c r="F6" s="16">
         <v>970318010</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="47">
+      <c r="H6" s="46">
         <v>2</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="46" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1355,13 +1380,13 @@
       <c r="F7" s="16">
         <v>972696048</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H7" s="46">
         <v>2</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="46" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1382,13 +1407,13 @@
       <c r="F8" s="15">
         <v>994455997</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="46">
         <v>2</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="46" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1409,13 +1434,13 @@
       <c r="F9" s="16">
         <v>982388953</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="47">
+      <c r="H9" s="46">
         <v>2</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="46" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1436,473 +1461,473 @@
       <c r="F10" s="20">
         <v>942176798</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="47">
         <v>3</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
-        <v>23</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="20">
-        <v>959692129</v>
+      <c r="A11" s="21">
+        <v>4</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="25">
+        <v>935212401</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="H11" s="48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" s="48" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22">
+    <row r="12" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
+        <v>7</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="26">
+        <v>996998808</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="48">
         <v>4</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
+      <c r="I12" s="48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
+        <v>11</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="25">
+        <v>994955279</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="48">
+        <v>4</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <v>13</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="26">
+        <v>946712465</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="48">
+        <v>4</v>
+      </c>
+      <c r="I14" s="85" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27">
         <v>19</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="31">
+        <v>998238959</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="49">
+        <v>5</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27">
+        <v>25</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="32">
+        <v>983315423</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="49">
+        <v>5</v>
+      </c>
+      <c r="I16" s="49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27">
+        <v>10</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="32">
+        <v>993096628</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="49">
+        <v>5</v>
+      </c>
+      <c r="I17" s="49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="33">
+        <v>12</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="36">
+        <v>997334727</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="50">
+        <v>6</v>
+      </c>
+      <c r="I18" s="50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33">
+        <v>3</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="36">
+        <v>926569656</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="50">
+        <v>6</v>
+      </c>
+      <c r="I19" s="50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="33">
         <v>20</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="26">
-        <v>935212401</v>
-      </c>
-      <c r="G12" s="43" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="38">
+        <v>976124099</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="50">
+        <v>6</v>
+      </c>
+      <c r="I20" s="50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33">
         <v>22</v>
       </c>
-      <c r="H12" s="49">
-        <v>4</v>
-      </c>
-      <c r="I12" s="49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22">
+      <c r="B21" s="37"/>
+      <c r="C21" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="36">
+        <v>939802475</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="50">
+        <v>6</v>
+      </c>
+      <c r="I21" s="50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="51">
+        <v>1</v>
+      </c>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="27">
-        <v>996998808</v>
-      </c>
-      <c r="G13" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="49">
-        <v>4</v>
-      </c>
-      <c r="I13" s="49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22">
+      <c r="D22" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="54">
+        <v>948098851</v>
+      </c>
+      <c r="G22" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="56">
+        <v>7</v>
+      </c>
+      <c r="I22" s="93" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="57">
+        <v>9</v>
+      </c>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="60">
+        <v>934505545</v>
+      </c>
+      <c r="G23" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="62">
+        <v>8</v>
+      </c>
+      <c r="I23" s="62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="63">
+        <v>24</v>
+      </c>
+      <c r="B24" s="64"/>
+      <c r="C24" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="67">
+        <v>948901251</v>
+      </c>
+      <c r="G24" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="69">
+        <v>9</v>
+      </c>
+      <c r="I24" s="69" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="70">
+        <v>2</v>
+      </c>
+      <c r="B25" s="71"/>
+      <c r="C25" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="26">
-        <v>994955279</v>
-      </c>
-      <c r="G14" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="49">
-        <v>4</v>
-      </c>
-      <c r="I14" s="86" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22">
+      <c r="D25" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="27">
-        <v>946712465</v>
-      </c>
-      <c r="G15" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="49">
-        <v>4</v>
-      </c>
-      <c r="I15" s="49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28">
-        <v>19</v>
-      </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="32">
-        <v>998238959</v>
-      </c>
-      <c r="G16" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="50">
-        <v>5</v>
-      </c>
-      <c r="I16" s="50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28">
-        <v>25</v>
-      </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="31" t="s">
+      <c r="F25" s="74">
+        <v>947375704</v>
+      </c>
+      <c r="G25" s="75" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="76">
+        <v>10</v>
+      </c>
+      <c r="I25" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="77">
+        <v>14</v>
+      </c>
+      <c r="B26" s="78"/>
+      <c r="C26" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="33">
-        <v>983315423</v>
-      </c>
-      <c r="G17" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" s="50">
-        <v>5</v>
-      </c>
-      <c r="I17" s="50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28">
-        <v>10</v>
-      </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="33">
-        <v>993096628</v>
-      </c>
-      <c r="G18" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" s="50">
-        <v>5</v>
-      </c>
-      <c r="I18" s="50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="34">
+      <c r="E26" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="81">
+        <v>914342202</v>
+      </c>
+      <c r="G26" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="83">
+        <v>11</v>
+      </c>
+      <c r="I26" s="83" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="86">
+        <v>23</v>
+      </c>
+      <c r="B27" s="87"/>
+      <c r="C27" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="90">
+        <v>959692129</v>
+      </c>
+      <c r="G27" s="91" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="92">
         <v>12</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="37">
-        <v>997334727</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="51">
-        <v>6</v>
-      </c>
-      <c r="I19" s="51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34">
-        <v>3</v>
-      </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="37">
-        <v>926569656</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="51">
-        <v>6</v>
-      </c>
-      <c r="I20" s="51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="34">
-        <v>20</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="39">
-        <v>976124099</v>
-      </c>
-      <c r="G21" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="51">
-        <v>6</v>
-      </c>
-      <c r="I21" s="51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34">
-        <v>22</v>
-      </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="37">
-        <v>939802475</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="51">
-        <v>6</v>
-      </c>
-      <c r="I22" s="87" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52">
-        <v>1</v>
-      </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="54" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="54" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="55">
-        <v>948098851</v>
-      </c>
-      <c r="G23" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="57">
-        <v>7</v>
-      </c>
-      <c r="I23" s="57" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="58">
-        <v>9</v>
-      </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="61">
-        <v>934505545</v>
-      </c>
-      <c r="G24" s="62" t="s">
-        <v>42</v>
-      </c>
-      <c r="H24" s="63">
-        <v>8</v>
-      </c>
-      <c r="I24" s="63" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="64">
-        <v>24</v>
-      </c>
-      <c r="B25" s="65"/>
-      <c r="C25" s="66" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="67" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="67" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="68">
-        <v>948901251</v>
-      </c>
-      <c r="G25" s="69" t="s">
-        <v>100</v>
-      </c>
-      <c r="H25" s="70">
-        <v>9</v>
-      </c>
-      <c r="I25" s="70" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="71">
-        <v>2</v>
-      </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="75">
-        <v>947375704</v>
-      </c>
-      <c r="G26" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="77">
-        <v>10</v>
-      </c>
-      <c r="I26" s="77" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="78">
-        <v>14</v>
-      </c>
-      <c r="B27" s="79"/>
-      <c r="C27" s="80" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="82">
-        <v>914342202</v>
-      </c>
-      <c r="G27" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="84">
-        <v>11</v>
-      </c>
-      <c r="I27" s="84" t="s">
-        <v>116</v>
+      <c r="I27" s="92" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>